<commit_message>
updated the Excel sheet with APIs
</commit_message>
<xml_diff>
--- a/WebAdmin API's .xlsx
+++ b/WebAdmin API's .xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="95">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="112" uniqueCount="97">
   <si>
     <t>No of Orders</t>
   </si>
@@ -301,6 +301,12 @@
   </si>
   <si>
     <t>Services</t>
+  </si>
+  <si>
+    <t>Dashboard</t>
+  </si>
+  <si>
+    <t>GetDashboardRecentOrdersByStatus</t>
   </si>
 </sst>
 </file>
@@ -540,7 +546,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -580,6 +586,30 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -590,25 +620,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
@@ -620,21 +632,12 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1079,7 +1082,7 @@
         <v>14</v>
       </c>
       <c r="D15" s="2"/>
-      <c r="E15" s="19" t="s">
+      <c r="E15" s="27" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1091,7 +1094,7 @@
         <v>15</v>
       </c>
       <c r="D16" s="2"/>
-      <c r="E16" s="19"/>
+      <c r="E16" s="27"/>
     </row>
     <row r="17" spans="2:5">
       <c r="B17" s="15"/>
@@ -1115,7 +1118,7 @@
       <c r="D19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="19" t="s">
+      <c r="E19" s="27" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1125,7 +1128,7 @@
       <c r="D20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="19"/>
+      <c r="E20" s="27"/>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" s="15"/>
@@ -1133,7 +1136,7 @@
       <c r="D21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="19"/>
+      <c r="E21" s="27"/>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" s="15"/>
@@ -1247,7 +1250,7 @@
       <c r="D34" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E34" s="20" t="s">
+      <c r="E34" s="28" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1257,7 +1260,7 @@
       <c r="D35" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E35" s="20"/>
+      <c r="E35" s="28"/>
     </row>
     <row r="36" spans="2:5">
       <c r="B36" s="15"/>
@@ -1265,7 +1268,7 @@
       <c r="D36" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E36" s="20"/>
+      <c r="E36" s="28"/>
     </row>
     <row r="37" spans="2:5">
       <c r="B37" s="15"/>
@@ -1273,7 +1276,7 @@
       <c r="D37" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E37" s="20"/>
+      <c r="E37" s="28"/>
     </row>
     <row r="38" spans="2:5">
       <c r="B38" s="15"/>
@@ -1313,7 +1316,7 @@
       <c r="D42" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E42" s="21" t="s">
+      <c r="E42" s="29" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1323,7 +1326,7 @@
       <c r="D43" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E43" s="21"/>
+      <c r="E43" s="29"/>
     </row>
     <row r="44" spans="2:5">
       <c r="B44" s="15"/>
@@ -1331,7 +1334,7 @@
       <c r="D44" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E44" s="21"/>
+      <c r="E44" s="29"/>
     </row>
     <row r="45" spans="2:5">
       <c r="B45" s="15"/>
@@ -1339,7 +1342,7 @@
       <c r="D45" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E45" s="21"/>
+      <c r="E45" s="29"/>
     </row>
     <row r="46" spans="2:5">
       <c r="B46" s="15"/>
@@ -1363,7 +1366,7 @@
       <c r="D48" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E48" s="21" t="s">
+      <c r="E48" s="29" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1373,7 +1376,7 @@
       <c r="D49" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E49" s="21"/>
+      <c r="E49" s="29"/>
     </row>
     <row r="50" spans="2:5">
       <c r="B50" s="15"/>
@@ -1381,7 +1384,7 @@
       <c r="D50" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E50" s="21"/>
+      <c r="E50" s="29"/>
     </row>
     <row r="51" spans="2:5">
       <c r="B51" s="15"/>
@@ -1389,7 +1392,7 @@
       <c r="D51" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E51" s="21"/>
+      <c r="E51" s="29"/>
     </row>
     <row r="52" spans="2:5">
       <c r="B52" s="15"/>
@@ -1413,7 +1416,7 @@
       <c r="D54" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E54" s="21" t="s">
+      <c r="E54" s="29" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1423,7 +1426,7 @@
       <c r="D55" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E55" s="21"/>
+      <c r="E55" s="29"/>
     </row>
     <row r="56" spans="2:5">
       <c r="B56" s="15"/>
@@ -1431,7 +1434,7 @@
       <c r="D56" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E56" s="21"/>
+      <c r="E56" s="29"/>
     </row>
     <row r="57" spans="2:5">
       <c r="B57" s="15"/>
@@ -1439,7 +1442,7 @@
       <c r="D57" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E57" s="21"/>
+      <c r="E57" s="29"/>
     </row>
     <row r="58" spans="2:5">
       <c r="B58" s="15"/>
@@ -1603,7 +1606,7 @@
       <c r="D75" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E75" s="20" t="s">
+      <c r="E75" s="28" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1613,7 +1616,7 @@
       <c r="D76" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E76" s="20"/>
+      <c r="E76" s="28"/>
     </row>
     <row r="77" spans="2:5">
       <c r="B77" s="15"/>
@@ -1621,7 +1624,7 @@
       <c r="D77" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E77" s="20"/>
+      <c r="E77" s="28"/>
     </row>
     <row r="78" spans="2:5">
       <c r="B78" s="15">
@@ -1708,14 +1711,14 @@
       <c r="E86" s="18"/>
     </row>
     <row r="87" spans="2:5">
-      <c r="B87" s="22">
+      <c r="B87" s="19">
         <v>33</v>
       </c>
       <c r="C87" s="2" t="s">
         <v>80</v>
       </c>
       <c r="D87" s="2"/>
-      <c r="E87" s="23"/>
+      <c r="E87" s="20"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -1736,212 +1739,224 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:F23"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="K10" sqref="K10"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="I13" sqref="I13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
-    <col min="2" max="2" width="8.88671875" style="26"/>
-    <col min="3" max="3" width="8.88671875" style="1"/>
-    <col min="4" max="4" width="18.5546875" style="28" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="18.5546875" style="28" customWidth="1"/>
+    <col min="2" max="2" width="8.88671875" style="22"/>
+    <col min="3" max="3" width="9.77734375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="31.33203125" style="24" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="18.5546875" style="24" customWidth="1"/>
     <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
-      <c r="D2" s="36" t="s">
+      <c r="D2" s="25" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="4" spans="2:6">
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="26" t="s">
         <v>93</v>
       </c>
-      <c r="C4" s="37" t="s">
+      <c r="C4" s="26" t="s">
         <v>86</v>
       </c>
-      <c r="D4" s="37" t="s">
+      <c r="D4" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="E4" s="37" t="s">
+      <c r="E4" s="26" t="s">
         <v>90</v>
       </c>
-      <c r="F4" s="37" t="s">
+      <c r="F4" s="26" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="5" spans="2:6">
-      <c r="B5" s="25">
+      <c r="B5" s="21">
         <v>1</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="30" t="s">
         <v>94</v>
       </c>
-      <c r="D5" s="27" t="s">
+      <c r="D5" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="E5" s="32"/>
-      <c r="F5" s="29" t="s">
+      <c r="E5" s="34" t="s">
+        <v>91</v>
+      </c>
+      <c r="F5" s="31" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="6" spans="2:6">
-      <c r="B6" s="25">
+      <c r="B6" s="21">
         <v>2</v>
       </c>
-      <c r="C6" s="24"/>
-      <c r="D6" s="27" t="s">
+      <c r="C6" s="30"/>
+      <c r="D6" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="33"/>
-      <c r="F6" s="30"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="32"/>
     </row>
     <row r="7" spans="2:6">
-      <c r="B7" s="25">
+      <c r="B7" s="21">
         <v>3</v>
       </c>
-      <c r="C7" s="24"/>
-      <c r="D7" s="27" t="s">
+      <c r="C7" s="30"/>
+      <c r="D7" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="E7" s="33"/>
-      <c r="F7" s="30"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="32"/>
     </row>
     <row r="8" spans="2:6">
-      <c r="B8" s="25">
+      <c r="B8" s="21">
         <v>4</v>
       </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="27" t="s">
+      <c r="C8" s="30"/>
+      <c r="D8" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="35" t="s">
-        <v>91</v>
-      </c>
-      <c r="F8" s="30"/>
+      <c r="E8" s="35"/>
+      <c r="F8" s="32"/>
     </row>
     <row r="9" spans="2:6">
-      <c r="B9" s="25">
+      <c r="B9" s="21">
         <v>5</v>
       </c>
-      <c r="C9" s="24"/>
-      <c r="D9" s="27" t="s">
+      <c r="C9" s="30"/>
+      <c r="D9" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="E9" s="33"/>
-      <c r="F9" s="30"/>
+      <c r="E9" s="35"/>
+      <c r="F9" s="32"/>
     </row>
     <row r="10" spans="2:6">
-      <c r="B10" s="25">
+      <c r="B10" s="21">
         <v>6</v>
       </c>
-      <c r="C10" s="24"/>
-      <c r="D10" s="27" t="s">
+      <c r="C10" s="30"/>
+      <c r="D10" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="E10" s="33"/>
-      <c r="F10" s="30"/>
+      <c r="E10" s="35"/>
+      <c r="F10" s="32"/>
     </row>
     <row r="11" spans="2:6">
-      <c r="B11" s="25">
+      <c r="B11" s="21">
         <v>7</v>
       </c>
-      <c r="C11" s="24"/>
-      <c r="D11" s="27" t="s">
+      <c r="C11" s="30"/>
+      <c r="D11" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="31"/>
+      <c r="E11" s="35"/>
+      <c r="F11" s="32"/>
     </row>
     <row r="12" spans="2:6">
-      <c r="B12" s="25"/>
-      <c r="C12" s="22"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
-      <c r="F12" s="2"/>
+      <c r="B12" s="21">
+        <v>8</v>
+      </c>
+      <c r="C12" s="34" t="s">
+        <v>95</v>
+      </c>
+      <c r="D12" s="23" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="35"/>
+      <c r="F12" s="32"/>
     </row>
     <row r="13" spans="2:6">
-      <c r="B13" s="25"/>
-      <c r="C13" s="22"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
-      <c r="F13" s="2"/>
+      <c r="B13" s="21">
+        <v>9</v>
+      </c>
+      <c r="C13" s="36"/>
+      <c r="D13" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="E13" s="36"/>
+      <c r="F13" s="33"/>
     </row>
     <row r="14" spans="2:6">
-      <c r="B14" s="25"/>
-      <c r="C14" s="22"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
+      <c r="B14" s="21"/>
+      <c r="C14" s="19"/>
+      <c r="D14" s="23"/>
+      <c r="E14" s="23"/>
       <c r="F14" s="2"/>
     </row>
     <row r="15" spans="2:6">
-      <c r="B15" s="25"/>
-      <c r="C15" s="22"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="19"/>
+      <c r="D15" s="23"/>
+      <c r="E15" s="23"/>
       <c r="F15" s="2"/>
     </row>
     <row r="16" spans="2:6">
-      <c r="B16" s="25"/>
-      <c r="C16" s="22"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
+      <c r="B16" s="21"/>
+      <c r="C16" s="19"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="2:6">
-      <c r="B17" s="25"/>
-      <c r="C17" s="22"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
+      <c r="B17" s="21"/>
+      <c r="C17" s="19"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="23"/>
       <c r="F17" s="2"/>
     </row>
     <row r="18" spans="2:6">
-      <c r="B18" s="25"/>
-      <c r="C18" s="22"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="19"/>
+      <c r="D18" s="23"/>
+      <c r="E18" s="23"/>
       <c r="F18" s="2"/>
     </row>
     <row r="19" spans="2:6">
-      <c r="B19" s="25"/>
-      <c r="C19" s="22"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
+      <c r="B19" s="21"/>
+      <c r="C19" s="19"/>
+      <c r="D19" s="23"/>
+      <c r="E19" s="23"/>
       <c r="F19" s="2"/>
     </row>
     <row r="20" spans="2:6">
-      <c r="B20" s="25"/>
-      <c r="C20" s="22"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
+      <c r="B20" s="21"/>
+      <c r="C20" s="19"/>
+      <c r="D20" s="23"/>
+      <c r="E20" s="23"/>
       <c r="F20" s="2"/>
     </row>
     <row r="21" spans="2:6">
-      <c r="B21" s="25"/>
-      <c r="C21" s="22"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
+      <c r="B21" s="21"/>
+      <c r="C21" s="19"/>
+      <c r="D21" s="23"/>
+      <c r="E21" s="23"/>
       <c r="F21" s="2"/>
     </row>
     <row r="22" spans="2:6">
-      <c r="B22" s="25"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="27"/>
-      <c r="E22" s="27"/>
+      <c r="B22" s="21"/>
+      <c r="C22" s="19"/>
+      <c r="D22" s="23"/>
+      <c r="E22" s="23"/>
       <c r="F22" s="2"/>
     </row>
     <row r="23" spans="2:6">
-      <c r="B23" s="25"/>
-      <c r="C23" s="22"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
+      <c r="B23" s="21"/>
+      <c r="C23" s="19"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="23"/>
       <c r="F23" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="4">
     <mergeCell ref="C5:C11"/>
-    <mergeCell ref="F5:F11"/>
+    <mergeCell ref="C12:C13"/>
+    <mergeCell ref="E5:E13"/>
+    <mergeCell ref="F5:F13"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F5" r:id="rId1"/>

</xml_diff>

<commit_message>
GetCustomerRatingsForOrders API- Not tested
</commit_message>
<xml_diff>
--- a/WebAdmin API's .xlsx
+++ b/WebAdmin API's .xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="115">
   <si>
     <t>No of Orders</t>
   </si>
@@ -351,10 +351,16 @@
     <t>Customer</t>
   </si>
   <si>
-    <t>GetAllCustomersByStatus</t>
-  </si>
-  <si>
-    <t>http://api.tasko.in/A1/</t>
+    <t>GetAllCustomersByStatus (New)</t>
+  </si>
+  <si>
+    <t>GetCustomerAddresses (AlredayExists)</t>
+  </si>
+  <si>
+    <t>GetCustomerDetails(AlredayExists)</t>
+  </si>
+  <si>
+    <t>GetCustomerOrders(AlredayExists)</t>
   </si>
 </sst>
 </file>
@@ -673,19 +679,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -1003,8 +1009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B1:H87"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+    <sheetView showGridLines="0" topLeftCell="A42" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54:E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1806,14 +1812,14 @@
   <dimension ref="B2:F35"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F31" sqref="F31:F32"/>
+      <selection activeCell="D35" sqref="D35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="8.85546875" style="22"/>
     <col min="3" max="3" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="31.28515625" style="24" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" style="24" customWidth="1"/>
     <col min="5" max="5" width="18.5703125" style="24" customWidth="1"/>
     <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
@@ -1844,13 +1850,13 @@
       <c r="B5" s="21">
         <v>1</v>
       </c>
-      <c r="C5" s="32" t="s">
+      <c r="C5" s="36" t="s">
         <v>94</v>
       </c>
       <c r="D5" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="E5" s="34" t="s">
+      <c r="E5" s="32" t="s">
         <v>91</v>
       </c>
       <c r="F5" s="37" t="s">
@@ -1861,90 +1867,90 @@
       <c r="B6" s="21">
         <v>2</v>
       </c>
-      <c r="C6" s="32"/>
+      <c r="C6" s="36"/>
       <c r="D6" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="36"/>
+      <c r="E6" s="33"/>
       <c r="F6" s="38"/>
     </row>
     <row r="7" spans="2:6">
       <c r="B7" s="21">
         <v>3</v>
       </c>
-      <c r="C7" s="32"/>
+      <c r="C7" s="36"/>
       <c r="D7" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="E7" s="36"/>
+      <c r="E7" s="33"/>
       <c r="F7" s="38"/>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" s="21">
         <v>4</v>
       </c>
-      <c r="C8" s="32"/>
+      <c r="C8" s="36"/>
       <c r="D8" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="36"/>
+      <c r="E8" s="33"/>
       <c r="F8" s="38"/>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" s="21">
         <v>5</v>
       </c>
-      <c r="C9" s="32"/>
+      <c r="C9" s="36"/>
       <c r="D9" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="E9" s="36"/>
+      <c r="E9" s="33"/>
       <c r="F9" s="38"/>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="21">
         <v>6</v>
       </c>
-      <c r="C10" s="32"/>
+      <c r="C10" s="36"/>
       <c r="D10" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="E10" s="36"/>
+      <c r="E10" s="33"/>
       <c r="F10" s="38"/>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" s="21">
         <v>7</v>
       </c>
-      <c r="C11" s="32"/>
+      <c r="C11" s="36"/>
       <c r="D11" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="E11" s="36"/>
+      <c r="E11" s="33"/>
       <c r="F11" s="38"/>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="21">
         <v>8</v>
       </c>
-      <c r="C12" s="34" t="s">
+      <c r="C12" s="32" t="s">
         <v>95</v>
       </c>
       <c r="D12" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="36"/>
+      <c r="E12" s="33"/>
       <c r="F12" s="38"/>
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="21">
         <v>9</v>
       </c>
-      <c r="C13" s="35"/>
+      <c r="C13" s="34"/>
       <c r="D13" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="E13" s="35"/>
+      <c r="E13" s="34"/>
       <c r="F13" s="39"/>
     </row>
     <row r="14" spans="2:6">
@@ -1958,13 +1964,13 @@
       <c r="B15" s="27">
         <v>10</v>
       </c>
-      <c r="C15" s="34" t="s">
+      <c r="C15" s="32" t="s">
         <v>97</v>
       </c>
       <c r="D15" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="E15" s="34" t="s">
+      <c r="E15" s="32" t="s">
         <v>91</v>
       </c>
       <c r="F15" s="37" t="s">
@@ -1975,49 +1981,49 @@
       <c r="B16" s="27">
         <v>11</v>
       </c>
-      <c r="C16" s="36"/>
+      <c r="C16" s="33"/>
       <c r="D16" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="E16" s="36"/>
+      <c r="E16" s="33"/>
       <c r="F16" s="38"/>
     </row>
     <row r="17" spans="2:6">
       <c r="B17" s="27">
         <v>12</v>
       </c>
-      <c r="C17" s="36"/>
+      <c r="C17" s="33"/>
       <c r="D17" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="E17" s="36"/>
+      <c r="E17" s="33"/>
       <c r="F17" s="38"/>
     </row>
     <row r="18" spans="2:6">
       <c r="B18" s="27">
         <v>13</v>
       </c>
-      <c r="C18" s="36"/>
+      <c r="C18" s="33"/>
       <c r="D18" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="E18" s="36"/>
+      <c r="E18" s="33"/>
       <c r="F18" s="38"/>
     </row>
     <row r="19" spans="2:6">
       <c r="B19" s="27">
         <v>14</v>
       </c>
-      <c r="C19" s="36"/>
+      <c r="C19" s="33"/>
       <c r="D19" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="35"/>
+      <c r="E19" s="34"/>
       <c r="F19" s="39"/>
     </row>
     <row r="20" spans="2:6">
       <c r="B20" s="27"/>
-      <c r="C20" s="36"/>
+      <c r="C20" s="33"/>
       <c r="D20" s="23"/>
       <c r="E20" s="23"/>
       <c r="F20" s="2"/>
@@ -2026,7 +2032,7 @@
       <c r="B21" s="27">
         <v>15</v>
       </c>
-      <c r="C21" s="36"/>
+      <c r="C21" s="33"/>
       <c r="D21" s="23" t="s">
         <v>102</v>
       </c>
@@ -2041,7 +2047,7 @@
       <c r="B22" s="27">
         <v>16</v>
       </c>
-      <c r="C22" s="36"/>
+      <c r="C22" s="33"/>
       <c r="D22" s="23" t="s">
         <v>103</v>
       </c>
@@ -2052,7 +2058,7 @@
       <c r="B23" s="27">
         <v>17</v>
       </c>
-      <c r="C23" s="36"/>
+      <c r="C23" s="33"/>
       <c r="D23" s="23" t="s">
         <v>104</v>
       </c>
@@ -2063,7 +2069,7 @@
       <c r="B24" s="27">
         <v>18</v>
       </c>
-      <c r="C24" s="36"/>
+      <c r="C24" s="33"/>
       <c r="D24" s="23" t="s">
         <v>105</v>
       </c>
@@ -2074,7 +2080,7 @@
       <c r="B25" s="27">
         <v>19</v>
       </c>
-      <c r="C25" s="36"/>
+      <c r="C25" s="33"/>
       <c r="D25" s="23" t="s">
         <v>104</v>
       </c>
@@ -2085,7 +2091,7 @@
       <c r="B26" s="27">
         <v>20</v>
       </c>
-      <c r="C26" s="35"/>
+      <c r="C26" s="34"/>
       <c r="D26" s="23" t="s">
         <v>107</v>
       </c>
@@ -2103,16 +2109,16 @@
       <c r="B28" s="27">
         <v>21</v>
       </c>
-      <c r="C28" s="32" t="s">
+      <c r="C28" s="36" t="s">
         <v>108</v>
       </c>
       <c r="D28" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="E28" s="32" t="s">
+      <c r="E28" s="36" t="s">
         <v>91</v>
       </c>
-      <c r="F28" s="33" t="s">
+      <c r="F28" s="35" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2120,16 +2126,16 @@
       <c r="B29" s="27">
         <v>22</v>
       </c>
-      <c r="C29" s="32"/>
+      <c r="C29" s="36"/>
       <c r="D29" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="E29" s="32"/>
-      <c r="F29" s="32"/>
+      <c r="E29" s="36"/>
+      <c r="F29" s="36"/>
     </row>
     <row r="30" spans="2:6">
       <c r="B30" s="27"/>
-      <c r="C30" s="34" t="s">
+      <c r="C30" s="32" t="s">
         <v>110</v>
       </c>
       <c r="D30" s="23"/>
@@ -2140,71 +2146,80 @@
       <c r="B31" s="27">
         <v>23</v>
       </c>
-      <c r="C31" s="36"/>
+      <c r="C31" s="33"/>
       <c r="D31" s="23" t="s">
         <v>111</v>
       </c>
       <c r="E31" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="F31" s="33" t="s">
-        <v>112</v>
-      </c>
+      <c r="F31" s="35"/>
     </row>
     <row r="32" spans="2:6">
       <c r="B32" s="27"/>
-      <c r="C32" s="36"/>
+      <c r="C32" s="33"/>
       <c r="D32" s="23"/>
       <c r="E32" s="23"/>
-      <c r="F32" s="32"/>
+      <c r="F32" s="36"/>
     </row>
     <row r="33" spans="2:6">
       <c r="B33" s="27"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="23"/>
-      <c r="E33" s="23"/>
+      <c r="C33" s="33"/>
+      <c r="D33" s="23" t="s">
+        <v>112</v>
+      </c>
+      <c r="E33" s="23" t="s">
+        <v>110</v>
+      </c>
       <c r="F33" s="2"/>
     </row>
     <row r="34" spans="2:6">
       <c r="B34" s="27"/>
-      <c r="C34" s="35"/>
-      <c r="D34" s="23"/>
-      <c r="E34" s="23"/>
+      <c r="C34" s="34"/>
+      <c r="D34" s="23" t="s">
+        <v>113</v>
+      </c>
+      <c r="E34" s="23" t="s">
+        <v>110</v>
+      </c>
       <c r="F34" s="2"/>
     </row>
     <row r="35" spans="2:6">
       <c r="B35" s="27"/>
       <c r="C35" s="19"/>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23"/>
+      <c r="D35" s="23" t="s">
+        <v>114</v>
+      </c>
+      <c r="E35" s="23" t="s">
+        <v>110</v>
+      </c>
       <c r="F35" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="C30:C34"/>
-    <mergeCell ref="F31:F32"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="E28:E29"/>
-    <mergeCell ref="F28:F29"/>
+    <mergeCell ref="E21:E26"/>
+    <mergeCell ref="F21:F26"/>
+    <mergeCell ref="C15:C26"/>
     <mergeCell ref="C5:C11"/>
     <mergeCell ref="C12:C13"/>
     <mergeCell ref="E5:E13"/>
     <mergeCell ref="F5:F13"/>
     <mergeCell ref="E15:E19"/>
     <mergeCell ref="F15:F19"/>
-    <mergeCell ref="E21:E26"/>
-    <mergeCell ref="F21:F26"/>
-    <mergeCell ref="C15:C26"/>
+    <mergeCell ref="C30:C34"/>
+    <mergeCell ref="F31:F32"/>
+    <mergeCell ref="C28:C29"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="F28:F29"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F5" r:id="rId1"/>
     <hyperlink ref="F15" r:id="rId2"/>
     <hyperlink ref="F21" r:id="rId3"/>
     <hyperlink ref="F28" r:id="rId4"/>
-    <hyperlink ref="F31" r:id="rId5"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId6"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
 

</xml_diff>

<commit_message>
updated list of apis in admin
</commit_message>
<xml_diff>
--- a/WebAdmin API's .xlsx
+++ b/WebAdmin API's .xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="161" uniqueCount="124">
   <si>
     <t>No of Orders</t>
   </si>
@@ -373,13 +373,28 @@
   </si>
   <si>
     <t>GetPaymentInvoice</t>
+  </si>
+  <si>
+    <t>GetCustomerRatingsForOrders(New)</t>
+  </si>
+  <si>
+    <t>GetCustomerOverview (New)</t>
+  </si>
+  <si>
+    <t>User</t>
+  </si>
+  <si>
+    <t>Login</t>
+  </si>
+  <si>
+    <t>GetUserDetails</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -401,6 +416,14 @@
       <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -612,7 +635,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -691,6 +714,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -701,6 +727,24 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
@@ -709,9 +753,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -719,19 +760,19 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1034,16 +1075,16 @@
       <selection activeCell="E54" sqref="E54:E57"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="8.88671875" style="1"/>
-    <col min="3" max="3" width="27.44140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="50.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="1"/>
+    <col min="3" max="3" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="50.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="15" thickBot="1"/>
-    <row r="2" spans="2:8" ht="15" thickBot="1">
+    <row r="1" spans="2:8" ht="15.75" thickBot="1"/>
+    <row r="2" spans="2:8" ht="15.75" thickBot="1">
       <c r="B2" s="13" t="s">
         <v>71</v>
       </c>
@@ -1097,7 +1138,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="7" spans="2:8" ht="28.8">
+    <row r="7" spans="2:8" ht="30">
       <c r="B7" s="15"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2" t="s">
@@ -1149,7 +1190,7 @@
       <c r="D12" s="2"/>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="2:8" ht="28.8">
+    <row r="13" spans="2:8" ht="45">
       <c r="B13" s="15">
         <v>2</v>
       </c>
@@ -1175,7 +1216,7 @@
         <v>14</v>
       </c>
       <c r="D15" s="2"/>
-      <c r="E15" s="32" t="s">
+      <c r="E15" s="33" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1187,7 +1228,7 @@
         <v>15</v>
       </c>
       <c r="D16" s="2"/>
-      <c r="E16" s="32"/>
+      <c r="E16" s="33"/>
     </row>
     <row r="17" spans="2:5">
       <c r="B17" s="15"/>
@@ -1211,7 +1252,7 @@
       <c r="D19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="32" t="s">
+      <c r="E19" s="33" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1221,7 +1262,7 @@
       <c r="D20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="32"/>
+      <c r="E20" s="33"/>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" s="15"/>
@@ -1229,7 +1270,7 @@
       <c r="D21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="32"/>
+      <c r="E21" s="33"/>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" s="15"/>
@@ -1293,7 +1334,7 @@
       <c r="D28" s="2"/>
       <c r="E28" s="4"/>
     </row>
-    <row r="29" spans="2:5" ht="57.6">
+    <row r="29" spans="2:5" ht="60">
       <c r="B29" s="15">
         <v>10</v>
       </c>
@@ -1343,7 +1384,7 @@
       <c r="D34" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E34" s="33" t="s">
+      <c r="E34" s="34" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1353,7 +1394,7 @@
       <c r="D35" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E35" s="33"/>
+      <c r="E35" s="34"/>
     </row>
     <row r="36" spans="2:5">
       <c r="B36" s="15"/>
@@ -1361,7 +1402,7 @@
       <c r="D36" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E36" s="33"/>
+      <c r="E36" s="34"/>
     </row>
     <row r="37" spans="2:5">
       <c r="B37" s="15"/>
@@ -1369,7 +1410,7 @@
       <c r="D37" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E37" s="33"/>
+      <c r="E37" s="34"/>
     </row>
     <row r="38" spans="2:5">
       <c r="B38" s="15"/>
@@ -1409,7 +1450,7 @@
       <c r="D42" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E42" s="34" t="s">
+      <c r="E42" s="35" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1419,7 +1460,7 @@
       <c r="D43" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E43" s="34"/>
+      <c r="E43" s="35"/>
     </row>
     <row r="44" spans="2:5">
       <c r="B44" s="15"/>
@@ -1427,7 +1468,7 @@
       <c r="D44" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E44" s="34"/>
+      <c r="E44" s="35"/>
     </row>
     <row r="45" spans="2:5">
       <c r="B45" s="15"/>
@@ -1435,7 +1476,7 @@
       <c r="D45" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E45" s="34"/>
+      <c r="E45" s="35"/>
     </row>
     <row r="46" spans="2:5">
       <c r="B46" s="15"/>
@@ -1459,7 +1500,7 @@
       <c r="D48" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E48" s="34" t="s">
+      <c r="E48" s="35" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1469,7 +1510,7 @@
       <c r="D49" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E49" s="34"/>
+      <c r="E49" s="35"/>
     </row>
     <row r="50" spans="2:5">
       <c r="B50" s="15"/>
@@ -1477,7 +1518,7 @@
       <c r="D50" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E50" s="34"/>
+      <c r="E50" s="35"/>
     </row>
     <row r="51" spans="2:5">
       <c r="B51" s="15"/>
@@ -1485,7 +1526,7 @@
       <c r="D51" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E51" s="34"/>
+      <c r="E51" s="35"/>
     </row>
     <row r="52" spans="2:5">
       <c r="B52" s="15"/>
@@ -1509,7 +1550,7 @@
       <c r="D54" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E54" s="34" t="s">
+      <c r="E54" s="35" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1519,7 +1560,7 @@
       <c r="D55" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E55" s="34"/>
+      <c r="E55" s="35"/>
     </row>
     <row r="56" spans="2:5">
       <c r="B56" s="15"/>
@@ -1527,7 +1568,7 @@
       <c r="D56" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E56" s="34"/>
+      <c r="E56" s="35"/>
     </row>
     <row r="57" spans="2:5">
       <c r="B57" s="15"/>
@@ -1535,7 +1576,7 @@
       <c r="D57" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E57" s="34"/>
+      <c r="E57" s="35"/>
     </row>
     <row r="58" spans="2:5">
       <c r="B58" s="15"/>
@@ -1559,7 +1600,7 @@
       <c r="D60" s="2"/>
       <c r="E60" s="4"/>
     </row>
-    <row r="61" spans="2:5" ht="28.8">
+    <row r="61" spans="2:5" ht="45">
       <c r="B61" s="15">
         <v>15</v>
       </c>
@@ -1625,7 +1666,7 @@
       <c r="D67" s="2"/>
       <c r="E67" s="4"/>
     </row>
-    <row r="68" spans="2:5" ht="57.6">
+    <row r="68" spans="2:5" ht="60">
       <c r="B68" s="15">
         <v>20</v>
       </c>
@@ -1699,7 +1740,7 @@
       <c r="D75" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E75" s="33" t="s">
+      <c r="E75" s="34" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1709,7 +1750,7 @@
       <c r="D76" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E76" s="33"/>
+      <c r="E76" s="34"/>
     </row>
     <row r="77" spans="2:5">
       <c r="B77" s="15"/>
@@ -1717,7 +1758,7 @@
       <c r="D77" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E77" s="33"/>
+      <c r="E77" s="34"/>
     </row>
     <row r="78" spans="2:5">
       <c r="B78" s="15">
@@ -1755,7 +1796,7 @@
       <c r="D81" s="2"/>
       <c r="E81" s="4"/>
     </row>
-    <row r="82" spans="2:5" ht="28.8">
+    <row r="82" spans="2:5" ht="30">
       <c r="B82" s="15">
         <v>29</v>
       </c>
@@ -1830,19 +1871,19 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B2:F54"/>
+  <dimension ref="B2:F58"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A21" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="J51" sqref="J51"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="K46" sqref="K46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="2" max="2" width="8.88671875" style="22"/>
-    <col min="3" max="3" width="9.6640625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="37.44140625" style="24" customWidth="1"/>
-    <col min="5" max="5" width="18.5546875" style="24" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" style="22"/>
+    <col min="3" max="3" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="37.42578125" style="24" customWidth="1"/>
+    <col min="5" max="5" width="18.5703125" style="24" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:6">
@@ -1871,16 +1912,16 @@
       <c r="B5" s="21">
         <v>1</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="45" t="s">
         <v>94</v>
       </c>
       <c r="D5" s="23" t="s">
         <v>81</v>
       </c>
-      <c r="E5" s="35" t="s">
+      <c r="E5" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="F5" s="38" t="s">
+      <c r="F5" s="39" t="s">
         <v>89</v>
       </c>
     </row>
@@ -1888,100 +1929,100 @@
       <c r="B6" s="21">
         <v>2</v>
       </c>
-      <c r="C6" s="39"/>
+      <c r="C6" s="45"/>
       <c r="D6" s="23" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="36"/>
-      <c r="F6" s="44"/>
+      <c r="E6" s="43"/>
+      <c r="F6" s="40"/>
     </row>
     <row r="7" spans="2:6">
       <c r="B7" s="21">
         <v>3</v>
       </c>
-      <c r="C7" s="39"/>
+      <c r="C7" s="45"/>
       <c r="D7" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="E7" s="36"/>
-      <c r="F7" s="44"/>
+      <c r="E7" s="43"/>
+      <c r="F7" s="40"/>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" s="21">
         <v>4</v>
       </c>
-      <c r="C8" s="39"/>
+      <c r="C8" s="45"/>
       <c r="D8" s="23" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="36"/>
-      <c r="F8" s="44"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="40"/>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" s="21">
         <v>5</v>
       </c>
-      <c r="C9" s="39"/>
+      <c r="C9" s="45"/>
       <c r="D9" s="23" t="s">
         <v>83</v>
       </c>
-      <c r="E9" s="36"/>
-      <c r="F9" s="44"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="40"/>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="21">
         <v>6</v>
       </c>
-      <c r="C10" s="39"/>
+      <c r="C10" s="45"/>
       <c r="D10" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="E10" s="36"/>
-      <c r="F10" s="44"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="40"/>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" s="21">
         <v>7</v>
       </c>
-      <c r="C11" s="39"/>
+      <c r="C11" s="45"/>
       <c r="D11" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="E11" s="36"/>
-      <c r="F11" s="44"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="40"/>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="21">
         <v>8</v>
       </c>
-      <c r="C12" s="35" t="s">
+      <c r="C12" s="42" t="s">
         <v>95</v>
       </c>
       <c r="D12" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="36"/>
-      <c r="F12" s="44"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="40"/>
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="29"/>
-      <c r="C13" s="36"/>
+      <c r="C13" s="43"/>
       <c r="D13" s="23" t="s">
         <v>115</v>
       </c>
-      <c r="E13" s="36"/>
-      <c r="F13" s="44"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="40"/>
     </row>
     <row r="14" spans="2:6">
       <c r="B14" s="21">
         <v>9</v>
       </c>
-      <c r="C14" s="37"/>
+      <c r="C14" s="44"/>
       <c r="D14" s="23" t="s">
         <v>96</v>
       </c>
-      <c r="E14" s="37"/>
-      <c r="F14" s="45"/>
+      <c r="E14" s="44"/>
+      <c r="F14" s="41"/>
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="21"/>
@@ -1994,16 +2035,16 @@
       <c r="B16" s="27">
         <v>10</v>
       </c>
-      <c r="C16" s="35" t="s">
+      <c r="C16" s="42" t="s">
         <v>97</v>
       </c>
       <c r="D16" s="23" t="s">
         <v>98</v>
       </c>
-      <c r="E16" s="35" t="s">
+      <c r="E16" s="42" t="s">
         <v>91</v>
       </c>
-      <c r="F16" s="38" t="s">
+      <c r="F16" s="39" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2011,49 +2052,49 @@
       <c r="B17" s="27">
         <v>11</v>
       </c>
-      <c r="C17" s="36"/>
+      <c r="C17" s="43"/>
       <c r="D17" s="23" t="s">
         <v>99</v>
       </c>
-      <c r="E17" s="36"/>
-      <c r="F17" s="44"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="40"/>
     </row>
     <row r="18" spans="2:6">
       <c r="B18" s="27">
         <v>12</v>
       </c>
-      <c r="C18" s="36"/>
+      <c r="C18" s="43"/>
       <c r="D18" s="28" t="s">
         <v>100</v>
       </c>
-      <c r="E18" s="36"/>
-      <c r="F18" s="44"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="40"/>
     </row>
     <row r="19" spans="2:6">
       <c r="B19" s="27">
         <v>13</v>
       </c>
-      <c r="C19" s="36"/>
+      <c r="C19" s="43"/>
       <c r="D19" s="23" t="s">
         <v>101</v>
       </c>
-      <c r="E19" s="36"/>
-      <c r="F19" s="44"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="40"/>
     </row>
     <row r="20" spans="2:6">
       <c r="B20" s="27">
         <v>14</v>
       </c>
-      <c r="C20" s="36"/>
+      <c r="C20" s="43"/>
       <c r="D20" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="E20" s="37"/>
-      <c r="F20" s="45"/>
+      <c r="E20" s="44"/>
+      <c r="F20" s="41"/>
     </row>
     <row r="21" spans="2:6">
       <c r="B21" s="27"/>
-      <c r="C21" s="36"/>
+      <c r="C21" s="43"/>
       <c r="D21" s="23"/>
       <c r="E21" s="23"/>
       <c r="F21" s="2"/>
@@ -2062,14 +2103,14 @@
       <c r="B22" s="27">
         <v>15</v>
       </c>
-      <c r="C22" s="36"/>
+      <c r="C22" s="43"/>
       <c r="D22" s="23" t="s">
         <v>102</v>
       </c>
-      <c r="E22" s="41" t="s">
+      <c r="E22" s="36" t="s">
         <v>97</v>
       </c>
-      <c r="F22" s="38" t="s">
+      <c r="F22" s="39" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2077,56 +2118,56 @@
       <c r="B23" s="27">
         <v>16</v>
       </c>
-      <c r="C23" s="36"/>
+      <c r="C23" s="43"/>
       <c r="D23" s="23" t="s">
         <v>103</v>
       </c>
-      <c r="E23" s="42"/>
-      <c r="F23" s="44"/>
+      <c r="E23" s="37"/>
+      <c r="F23" s="40"/>
     </row>
     <row r="24" spans="2:6">
       <c r="B24" s="27">
         <v>17</v>
       </c>
-      <c r="C24" s="36"/>
+      <c r="C24" s="43"/>
       <c r="D24" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="E24" s="42"/>
-      <c r="F24" s="44"/>
+      <c r="E24" s="37"/>
+      <c r="F24" s="40"/>
     </row>
     <row r="25" spans="2:6">
       <c r="B25" s="27">
         <v>18</v>
       </c>
-      <c r="C25" s="36"/>
+      <c r="C25" s="43"/>
       <c r="D25" s="23" t="s">
         <v>105</v>
       </c>
-      <c r="E25" s="42"/>
-      <c r="F25" s="44"/>
+      <c r="E25" s="37"/>
+      <c r="F25" s="40"/>
     </row>
     <row r="26" spans="2:6">
       <c r="B26" s="27">
         <v>19</v>
       </c>
-      <c r="C26" s="36"/>
+      <c r="C26" s="43"/>
       <c r="D26" s="23" t="s">
         <v>104</v>
       </c>
-      <c r="E26" s="42"/>
-      <c r="F26" s="44"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="40"/>
     </row>
     <row r="27" spans="2:6">
       <c r="B27" s="27">
         <v>20</v>
       </c>
-      <c r="C27" s="37"/>
+      <c r="C27" s="44"/>
       <c r="D27" s="23" t="s">
         <v>107</v>
       </c>
-      <c r="E27" s="43"/>
-      <c r="F27" s="45"/>
+      <c r="E27" s="38"/>
+      <c r="F27" s="41"/>
     </row>
     <row r="28" spans="2:6">
       <c r="B28" s="27"/>
@@ -2139,16 +2180,16 @@
       <c r="B29" s="27">
         <v>21</v>
       </c>
-      <c r="C29" s="39" t="s">
+      <c r="C29" s="45" t="s">
         <v>108</v>
       </c>
       <c r="D29" s="23" t="s">
         <v>109</v>
       </c>
-      <c r="E29" s="39" t="s">
+      <c r="E29" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="F29" s="40" t="s">
+      <c r="F29" s="46" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2156,16 +2197,16 @@
       <c r="B30" s="27">
         <v>22</v>
       </c>
-      <c r="C30" s="39"/>
+      <c r="C30" s="45"/>
       <c r="D30" s="23" t="s">
         <v>20</v>
       </c>
-      <c r="E30" s="39"/>
-      <c r="F30" s="39"/>
+      <c r="E30" s="45"/>
+      <c r="F30" s="45"/>
     </row>
     <row r="31" spans="2:6">
       <c r="B31" s="27"/>
-      <c r="C31" s="35" t="s">
+      <c r="C31" s="42" t="s">
         <v>110</v>
       </c>
       <c r="D31" s="23"/>
@@ -2176,7 +2217,7 @@
       <c r="B32" s="27">
         <v>23</v>
       </c>
-      <c r="C32" s="36"/>
+      <c r="C32" s="43"/>
       <c r="D32" s="23" t="s">
         <v>111</v>
       </c>
@@ -2189,29 +2230,29 @@
     </row>
     <row r="33" spans="2:6">
       <c r="B33" s="27"/>
-      <c r="C33" s="36"/>
+      <c r="C33" s="43"/>
       <c r="D33" s="23"/>
       <c r="E33" s="23"/>
       <c r="F33" s="31"/>
     </row>
     <row r="34" spans="2:6">
       <c r="B34" s="27"/>
-      <c r="C34" s="36"/>
+      <c r="C34" s="43"/>
       <c r="D34" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="E34" s="35" t="s">
+      <c r="E34" s="42" t="s">
         <v>110</v>
       </c>
       <c r="F34" s="2"/>
     </row>
     <row r="35" spans="2:6">
       <c r="B35" s="27"/>
-      <c r="C35" s="37"/>
+      <c r="C35" s="44"/>
       <c r="D35" s="23" t="s">
         <v>113</v>
       </c>
-      <c r="E35" s="36"/>
+      <c r="E35" s="43"/>
       <c r="F35" s="2"/>
     </row>
     <row r="36" spans="2:6">
@@ -2220,104 +2261,112 @@
       <c r="D36" s="23" t="s">
         <v>114</v>
       </c>
-      <c r="E36" s="37"/>
+      <c r="E36" s="44"/>
       <c r="F36" s="2"/>
     </row>
     <row r="37" spans="2:6">
       <c r="B37" s="29"/>
       <c r="C37" s="19"/>
-      <c r="D37" s="23"/>
-      <c r="E37" s="23"/>
+      <c r="D37" s="23" t="s">
+        <v>119</v>
+      </c>
+      <c r="E37" s="23" t="s">
+        <v>91</v>
+      </c>
       <c r="F37" s="2"/>
     </row>
     <row r="38" spans="2:6">
-      <c r="B38" s="29">
-        <v>24</v>
-      </c>
-      <c r="C38" s="35" t="s">
-        <v>116</v>
-      </c>
+      <c r="B38" s="32"/>
+      <c r="C38" s="47"/>
       <c r="D38" s="23" t="s">
-        <v>63</v>
-      </c>
-      <c r="E38" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="E38" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="F38" s="38" t="s">
-        <v>89</v>
-      </c>
+      <c r="F38" s="17"/>
     </row>
     <row r="39" spans="2:6">
-      <c r="B39" s="29">
-        <v>25</v>
-      </c>
-      <c r="C39" s="36"/>
-      <c r="D39" s="23" t="s">
-        <v>66</v>
-      </c>
-      <c r="E39" s="36"/>
-      <c r="F39" s="44"/>
+      <c r="B39" s="32"/>
+      <c r="C39" s="47"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="48"/>
+      <c r="F39" s="17"/>
     </row>
     <row r="40" spans="2:6">
-      <c r="B40" s="29">
-        <v>26</v>
-      </c>
-      <c r="C40" s="36"/>
-      <c r="D40" s="23" t="s">
-        <v>117</v>
-      </c>
-      <c r="E40" s="36"/>
-      <c r="F40" s="44"/>
+      <c r="B40" s="32"/>
+      <c r="C40" s="47"/>
+      <c r="D40" s="23"/>
+      <c r="E40" s="48"/>
+      <c r="F40" s="17"/>
     </row>
     <row r="41" spans="2:6">
-      <c r="B41" s="29">
-        <v>27</v>
-      </c>
-      <c r="C41" s="36"/>
-      <c r="D41" s="23" t="s">
-        <v>62</v>
-      </c>
-      <c r="E41" s="36"/>
-      <c r="F41" s="44"/>
+      <c r="B41" s="32"/>
+      <c r="C41" s="47"/>
+      <c r="D41" s="23"/>
+      <c r="E41" s="48"/>
+      <c r="F41" s="17"/>
     </row>
     <row r="42" spans="2:6">
       <c r="B42" s="29">
+        <v>24</v>
+      </c>
+      <c r="C42" s="42" t="s">
+        <v>116</v>
+      </c>
+      <c r="D42" s="23" t="s">
+        <v>63</v>
+      </c>
+      <c r="E42" s="42" t="s">
+        <v>91</v>
+      </c>
+      <c r="F42" s="39" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6">
+      <c r="B43" s="29">
+        <v>25</v>
+      </c>
+      <c r="C43" s="43"/>
+      <c r="D43" s="23" t="s">
+        <v>66</v>
+      </c>
+      <c r="E43" s="43"/>
+      <c r="F43" s="40"/>
+    </row>
+    <row r="44" spans="2:6">
+      <c r="B44" s="29">
+        <v>26</v>
+      </c>
+      <c r="C44" s="43"/>
+      <c r="D44" s="23" t="s">
+        <v>117</v>
+      </c>
+      <c r="E44" s="43"/>
+      <c r="F44" s="40"/>
+    </row>
+    <row r="45" spans="2:6">
+      <c r="B45" s="29">
+        <v>27</v>
+      </c>
+      <c r="C45" s="43"/>
+      <c r="D45" s="23" t="s">
+        <v>62</v>
+      </c>
+      <c r="E45" s="43"/>
+      <c r="F45" s="40"/>
+    </row>
+    <row r="46" spans="2:6">
+      <c r="B46" s="29">
         <v>28</v>
       </c>
-      <c r="C42" s="37"/>
-      <c r="D42" s="23" t="s">
+      <c r="C46" s="44"/>
+      <c r="D46" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="E42" s="37"/>
-      <c r="F42" s="45"/>
-    </row>
-    <row r="43" spans="2:6">
-      <c r="B43" s="29"/>
-      <c r="C43" s="19"/>
-      <c r="D43" s="23"/>
-      <c r="E43" s="23"/>
-      <c r="F43" s="2"/>
-    </row>
-    <row r="44" spans="2:6">
-      <c r="B44" s="29"/>
-      <c r="C44" s="19"/>
-      <c r="D44" s="23"/>
-      <c r="E44" s="23"/>
-      <c r="F44" s="2"/>
-    </row>
-    <row r="45" spans="2:6">
-      <c r="B45" s="29"/>
-      <c r="C45" s="19"/>
-      <c r="D45" s="23"/>
-      <c r="E45" s="23"/>
-      <c r="F45" s="2"/>
-    </row>
-    <row r="46" spans="2:6">
-      <c r="B46" s="29"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="23"/>
-      <c r="E46" s="23"/>
-      <c r="F46" s="2"/>
+      <c r="E46" s="44"/>
+      <c r="F46" s="41"/>
     </row>
     <row r="47" spans="2:6">
       <c r="B47" s="29"/>
@@ -2328,55 +2377,107 @@
     </row>
     <row r="48" spans="2:6">
       <c r="B48" s="29"/>
-      <c r="C48" s="19"/>
-      <c r="D48" s="23"/>
+      <c r="C48" s="49" t="s">
+        <v>121</v>
+      </c>
+      <c r="D48" s="23" t="s">
+        <v>54</v>
+      </c>
       <c r="E48" s="23"/>
       <c r="F48" s="2"/>
     </row>
     <row r="49" spans="2:6">
       <c r="B49" s="29"/>
-      <c r="C49" s="19"/>
-      <c r="D49" s="23"/>
+      <c r="C49" s="50"/>
+      <c r="D49" s="23" t="s">
+        <v>56</v>
+      </c>
       <c r="E49" s="23"/>
       <c r="F49" s="2"/>
     </row>
     <row r="50" spans="2:6">
       <c r="B50" s="29"/>
-      <c r="C50" s="19"/>
-      <c r="D50" s="23"/>
+      <c r="C50" s="50"/>
+      <c r="D50" s="23" t="s">
+        <v>60</v>
+      </c>
       <c r="E50" s="23"/>
-      <c r="F50" s="2"/>
+      <c r="F50" s="39" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="51" spans="2:6">
       <c r="B51" s="29"/>
-      <c r="C51" s="19"/>
-      <c r="D51" s="23"/>
+      <c r="C51" s="50"/>
+      <c r="D51" s="23" t="s">
+        <v>122</v>
+      </c>
       <c r="E51" s="23"/>
-      <c r="F51" s="2"/>
+      <c r="F51" s="40"/>
     </row>
     <row r="52" spans="2:6">
       <c r="B52" s="29"/>
-      <c r="C52" s="19"/>
-      <c r="D52" s="23"/>
+      <c r="C52" s="50"/>
+      <c r="D52" s="23" t="s">
+        <v>123</v>
+      </c>
       <c r="E52" s="23"/>
-      <c r="F52" s="2"/>
+      <c r="F52" s="40"/>
     </row>
     <row r="53" spans="2:6">
       <c r="B53" s="29"/>
-      <c r="C53" s="19"/>
+      <c r="C53" s="51"/>
       <c r="D53" s="23"/>
       <c r="E53" s="23"/>
-      <c r="F53" s="2"/>
+      <c r="F53" s="40"/>
     </row>
     <row r="54" spans="2:6">
       <c r="B54" s="29"/>
       <c r="C54" s="19"/>
       <c r="D54" s="23"/>
       <c r="E54" s="23"/>
-      <c r="F54" s="2"/>
+      <c r="F54" s="41"/>
+    </row>
+    <row r="55" spans="2:6">
+      <c r="B55" s="29"/>
+      <c r="C55" s="19"/>
+      <c r="D55" s="23"/>
+      <c r="E55" s="23"/>
+      <c r="F55" s="2"/>
+    </row>
+    <row r="56" spans="2:6">
+      <c r="B56" s="29"/>
+      <c r="C56" s="19"/>
+      <c r="D56" s="23"/>
+      <c r="E56" s="23"/>
+      <c r="F56" s="2"/>
+    </row>
+    <row r="57" spans="2:6">
+      <c r="B57" s="29"/>
+      <c r="C57" s="19"/>
+      <c r="D57" s="23"/>
+      <c r="E57" s="23"/>
+      <c r="F57" s="2"/>
+    </row>
+    <row r="58" spans="2:6">
+      <c r="B58" s="29"/>
+      <c r="C58" s="19"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="23"/>
+      <c r="F58" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="19">
+    <mergeCell ref="E42:E46"/>
+    <mergeCell ref="F42:F46"/>
+    <mergeCell ref="C42:C46"/>
+    <mergeCell ref="F50:F54"/>
+    <mergeCell ref="C48:C53"/>
+    <mergeCell ref="C31:C35"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="E34:E36"/>
     <mergeCell ref="E22:E27"/>
     <mergeCell ref="F22:F27"/>
     <mergeCell ref="C16:C27"/>
@@ -2386,14 +2487,6 @@
     <mergeCell ref="F5:F14"/>
     <mergeCell ref="E16:E20"/>
     <mergeCell ref="F16:F20"/>
-    <mergeCell ref="C31:C35"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="E34:E36"/>
-    <mergeCell ref="E38:E42"/>
-    <mergeCell ref="F38:F42"/>
-    <mergeCell ref="C38:C42"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F5" r:id="rId1"/>
@@ -2401,10 +2494,11 @@
     <hyperlink ref="F22" r:id="rId3"/>
     <hyperlink ref="F29" r:id="rId4"/>
     <hyperlink ref="F32" r:id="rId5"/>
-    <hyperlink ref="F38" r:id="rId6"/>
+    <hyperlink ref="F42" r:id="rId6"/>
+    <hyperlink ref="F50" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId7"/>
+  <pageSetup orientation="portrait" r:id="rId8"/>
 </worksheet>
 </file>
 
@@ -2414,7 +2508,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Release notes updated in Excel Sheet with date
</commit_message>
<xml_diff>
--- a/WebAdmin API's .xlsx
+++ b/WebAdmin API's .xlsx
@@ -4,19 +4,19 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="108" windowWidth="14808" windowHeight="8016" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
     <sheet name="WebAdmin" sheetId="2" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Releases" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="125725"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="130">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="171" uniqueCount="135">
   <si>
     <t>No of Orders</t>
   </si>
@@ -406,6 +406,21 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>RC2</t>
+  </si>
+  <si>
+    <t>Candidate Name</t>
+  </si>
+  <si>
+    <t>Release Date</t>
+  </si>
+  <si>
+    <t>Dec 20th 2016</t>
+  </si>
+  <si>
+    <t>RC1</t>
   </si>
 </sst>
 </file>
@@ -743,7 +758,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="65">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -816,48 +831,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -875,9 +848,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
@@ -902,6 +872,52 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1344,7 +1360,7 @@
         <v>14</v>
       </c>
       <c r="D15" s="2"/>
-      <c r="E15" s="30" t="s">
+      <c r="E15" s="49" t="s">
         <v>69</v>
       </c>
     </row>
@@ -1356,7 +1372,7 @@
         <v>15</v>
       </c>
       <c r="D16" s="2"/>
-      <c r="E16" s="30"/>
+      <c r="E16" s="49"/>
     </row>
     <row r="17" spans="2:5">
       <c r="B17" s="15"/>
@@ -1380,7 +1396,7 @@
       <c r="D19" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="30" t="s">
+      <c r="E19" s="49" t="s">
         <v>70</v>
       </c>
     </row>
@@ -1390,7 +1406,7 @@
       <c r="D20" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="E20" s="30"/>
+      <c r="E20" s="49"/>
     </row>
     <row r="21" spans="2:5">
       <c r="B21" s="15"/>
@@ -1398,7 +1414,7 @@
       <c r="D21" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E21" s="30"/>
+      <c r="E21" s="49"/>
     </row>
     <row r="22" spans="2:5">
       <c r="B22" s="15"/>
@@ -1512,7 +1528,7 @@
       <c r="D34" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="E34" s="31" t="s">
+      <c r="E34" s="50" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1522,7 +1538,7 @@
       <c r="D35" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="E35" s="31"/>
+      <c r="E35" s="50"/>
     </row>
     <row r="36" spans="2:5">
       <c r="B36" s="15"/>
@@ -1530,7 +1546,7 @@
       <c r="D36" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="E36" s="31"/>
+      <c r="E36" s="50"/>
     </row>
     <row r="37" spans="2:5">
       <c r="B37" s="15"/>
@@ -1538,7 +1554,7 @@
       <c r="D37" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="E37" s="31"/>
+      <c r="E37" s="50"/>
     </row>
     <row r="38" spans="2:5">
       <c r="B38" s="15"/>
@@ -1578,7 +1594,7 @@
       <c r="D42" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="E42" s="32" t="s">
+      <c r="E42" s="51" t="s">
         <v>35</v>
       </c>
     </row>
@@ -1588,7 +1604,7 @@
       <c r="D43" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="E43" s="32"/>
+      <c r="E43" s="51"/>
     </row>
     <row r="44" spans="2:5">
       <c r="B44" s="15"/>
@@ -1596,7 +1612,7 @@
       <c r="D44" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="E44" s="32"/>
+      <c r="E44" s="51"/>
     </row>
     <row r="45" spans="2:5">
       <c r="B45" s="15"/>
@@ -1604,7 +1620,7 @@
       <c r="D45" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="E45" s="32"/>
+      <c r="E45" s="51"/>
     </row>
     <row r="46" spans="2:5">
       <c r="B46" s="15"/>
@@ -1628,7 +1644,7 @@
       <c r="D48" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="E48" s="32" t="s">
+      <c r="E48" s="51" t="s">
         <v>41</v>
       </c>
     </row>
@@ -1638,7 +1654,7 @@
       <c r="D49" s="2" t="s">
         <v>39</v>
       </c>
-      <c r="E49" s="32"/>
+      <c r="E49" s="51"/>
     </row>
     <row r="50" spans="2:5">
       <c r="B50" s="15"/>
@@ -1646,7 +1662,7 @@
       <c r="D50" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="E50" s="32"/>
+      <c r="E50" s="51"/>
     </row>
     <row r="51" spans="2:5">
       <c r="B51" s="15"/>
@@ -1654,7 +1670,7 @@
       <c r="D51" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="E51" s="32"/>
+      <c r="E51" s="51"/>
     </row>
     <row r="52" spans="2:5">
       <c r="B52" s="15"/>
@@ -1678,7 +1694,7 @@
       <c r="D54" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="E54" s="32" t="s">
+      <c r="E54" s="51" t="s">
         <v>46</v>
       </c>
     </row>
@@ -1688,7 +1704,7 @@
       <c r="D55" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="E55" s="32"/>
+      <c r="E55" s="51"/>
     </row>
     <row r="56" spans="2:5">
       <c r="B56" s="15"/>
@@ -1696,7 +1712,7 @@
       <c r="D56" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="E56" s="32"/>
+      <c r="E56" s="51"/>
     </row>
     <row r="57" spans="2:5">
       <c r="B57" s="15"/>
@@ -1704,7 +1720,7 @@
       <c r="D57" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="E57" s="32"/>
+      <c r="E57" s="51"/>
     </row>
     <row r="58" spans="2:5">
       <c r="B58" s="15"/>
@@ -1868,7 +1884,7 @@
       <c r="D75" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="E75" s="31" t="s">
+      <c r="E75" s="50" t="s">
         <v>19</v>
       </c>
     </row>
@@ -1878,7 +1894,7 @@
       <c r="D76" s="2" t="s">
         <v>65</v>
       </c>
-      <c r="E76" s="31"/>
+      <c r="E76" s="50"/>
     </row>
     <row r="77" spans="2:5">
       <c r="B77" s="15"/>
@@ -1886,7 +1902,7 @@
       <c r="D77" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="E77" s="31"/>
+      <c r="E77" s="50"/>
     </row>
     <row r="78" spans="2:5">
       <c r="B78" s="15">
@@ -2001,7 +2017,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="B2:M50"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
@@ -2041,16 +2057,16 @@
       <c r="B5" s="21">
         <v>1</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="61" t="s">
         <v>94</v>
       </c>
-      <c r="D5" s="46" t="s">
+      <c r="D5" s="32" t="s">
         <v>81</v>
       </c>
-      <c r="E5" s="33" t="s">
+      <c r="E5" s="54" t="s">
         <v>91</v>
       </c>
-      <c r="F5" s="36" t="s">
+      <c r="F5" s="55" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2058,117 +2074,117 @@
       <c r="B6" s="21">
         <v>2</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="46" t="s">
+      <c r="C6" s="61"/>
+      <c r="D6" s="32" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="34"/>
-      <c r="F6" s="37"/>
+      <c r="E6" s="52"/>
+      <c r="F6" s="59"/>
     </row>
     <row r="7" spans="2:6">
       <c r="B7" s="29">
         <v>3</v>
       </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="46" t="s">
+      <c r="C7" s="61"/>
+      <c r="D7" s="32" t="s">
         <v>82</v>
       </c>
-      <c r="E7" s="34"/>
-      <c r="F7" s="37"/>
+      <c r="E7" s="52"/>
+      <c r="F7" s="59"/>
     </row>
     <row r="8" spans="2:6">
       <c r="B8" s="29">
         <v>4</v>
       </c>
-      <c r="C8" s="39"/>
-      <c r="D8" s="46" t="s">
+      <c r="C8" s="61"/>
+      <c r="D8" s="32" t="s">
         <v>53</v>
       </c>
-      <c r="E8" s="34"/>
-      <c r="F8" s="37"/>
+      <c r="E8" s="52"/>
+      <c r="F8" s="59"/>
     </row>
     <row r="9" spans="2:6">
       <c r="B9" s="29">
         <v>5</v>
       </c>
-      <c r="C9" s="39"/>
-      <c r="D9" s="46" t="s">
+      <c r="C9" s="61"/>
+      <c r="D9" s="32" t="s">
         <v>83</v>
       </c>
-      <c r="E9" s="34"/>
-      <c r="F9" s="37"/>
+      <c r="E9" s="52"/>
+      <c r="F9" s="59"/>
     </row>
     <row r="10" spans="2:6">
       <c r="B10" s="29">
         <v>6</v>
       </c>
-      <c r="C10" s="39"/>
-      <c r="D10" s="46" t="s">
+      <c r="C10" s="61"/>
+      <c r="D10" s="32" t="s">
         <v>84</v>
       </c>
-      <c r="E10" s="34"/>
-      <c r="F10" s="37"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="59"/>
     </row>
     <row r="11" spans="2:6">
       <c r="B11" s="29">
         <v>7</v>
       </c>
-      <c r="C11" s="39"/>
-      <c r="D11" s="46" t="s">
+      <c r="C11" s="61"/>
+      <c r="D11" s="32" t="s">
         <v>85</v>
       </c>
-      <c r="E11" s="34"/>
-      <c r="F11" s="37"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="59"/>
     </row>
     <row r="12" spans="2:6">
       <c r="B12" s="29">
         <v>8</v>
       </c>
-      <c r="C12" s="33" t="s">
+      <c r="C12" s="54" t="s">
         <v>95</v>
       </c>
-      <c r="D12" s="46" t="s">
+      <c r="D12" s="32" t="s">
         <v>12</v>
       </c>
-      <c r="E12" s="34"/>
-      <c r="F12" s="37"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="59"/>
     </row>
     <row r="13" spans="2:6">
       <c r="B13" s="29">
         <v>9</v>
       </c>
-      <c r="C13" s="34"/>
-      <c r="D13" s="46" t="s">
+      <c r="C13" s="52"/>
+      <c r="D13" s="32" t="s">
         <v>114</v>
       </c>
-      <c r="E13" s="34"/>
-      <c r="F13" s="37"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="59"/>
     </row>
     <row r="14" spans="2:6">
       <c r="B14" s="29">
         <v>10</v>
       </c>
-      <c r="C14" s="35"/>
-      <c r="D14" s="46" t="s">
+      <c r="C14" s="53"/>
+      <c r="D14" s="32" t="s">
         <v>96</v>
       </c>
-      <c r="E14" s="35"/>
-      <c r="F14" s="38"/>
+      <c r="E14" s="53"/>
+      <c r="F14" s="60"/>
     </row>
     <row r="15" spans="2:6">
       <c r="B15" s="29">
         <v>11</v>
       </c>
-      <c r="C15" s="33" t="s">
+      <c r="C15" s="54" t="s">
         <v>97</v>
       </c>
-      <c r="D15" s="46" t="s">
+      <c r="D15" s="32" t="s">
         <v>98</v>
       </c>
-      <c r="E15" s="33" t="s">
+      <c r="E15" s="54" t="s">
         <v>91</v>
       </c>
-      <c r="F15" s="36" t="s">
+      <c r="F15" s="55" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2176,58 +2192,58 @@
       <c r="B16" s="29">
         <v>12</v>
       </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="46" t="s">
+      <c r="C16" s="52"/>
+      <c r="D16" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="E16" s="34"/>
-      <c r="F16" s="37"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="59"/>
     </row>
     <row r="17" spans="2:13">
       <c r="B17" s="29">
         <v>13</v>
       </c>
-      <c r="C17" s="34"/>
-      <c r="D17" s="47" t="s">
+      <c r="C17" s="52"/>
+      <c r="D17" s="33" t="s">
         <v>100</v>
       </c>
-      <c r="E17" s="34"/>
-      <c r="F17" s="37"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="59"/>
     </row>
     <row r="18" spans="2:13">
       <c r="B18" s="29">
         <v>14</v>
       </c>
-      <c r="C18" s="34"/>
-      <c r="D18" s="46" t="s">
+      <c r="C18" s="52"/>
+      <c r="D18" s="32" t="s">
         <v>101</v>
       </c>
-      <c r="E18" s="34"/>
-      <c r="F18" s="37"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="59"/>
     </row>
     <row r="19" spans="2:13">
       <c r="B19" s="29">
         <v>15</v>
       </c>
-      <c r="C19" s="34"/>
-      <c r="D19" s="46" t="s">
+      <c r="C19" s="52"/>
+      <c r="D19" s="32" t="s">
         <v>27</v>
       </c>
-      <c r="E19" s="35"/>
-      <c r="F19" s="38"/>
+      <c r="E19" s="53"/>
+      <c r="F19" s="60"/>
     </row>
     <row r="20" spans="2:13">
       <c r="B20" s="29">
         <v>16</v>
       </c>
-      <c r="C20" s="34"/>
-      <c r="D20" s="45" t="s">
+      <c r="C20" s="52"/>
+      <c r="D20" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="E20" s="41" t="s">
+      <c r="E20" s="56" t="s">
         <v>97</v>
       </c>
-      <c r="F20" s="36" t="s">
+      <c r="F20" s="55" t="s">
         <v>106</v>
       </c>
     </row>
@@ -2235,102 +2251,102 @@
       <c r="B21" s="29">
         <v>17</v>
       </c>
-      <c r="C21" s="34"/>
-      <c r="D21" s="45" t="s">
+      <c r="C21" s="52"/>
+      <c r="D21" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="E21" s="42"/>
-      <c r="F21" s="37"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="59"/>
     </row>
     <row r="22" spans="2:13">
       <c r="B22" s="29">
         <v>18</v>
       </c>
-      <c r="C22" s="34"/>
-      <c r="D22" s="45" t="s">
+      <c r="C22" s="52"/>
+      <c r="D22" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="E22" s="42"/>
-      <c r="F22" s="37"/>
-      <c r="J22" s="51"/>
-      <c r="K22" s="52"/>
-      <c r="L22" s="53"/>
-      <c r="M22" s="54"/>
+      <c r="E22" s="57"/>
+      <c r="F22" s="59"/>
+      <c r="J22" s="36"/>
+      <c r="K22" s="37"/>
+      <c r="L22" s="38"/>
+      <c r="M22" s="39"/>
     </row>
     <row r="23" spans="2:13">
       <c r="B23" s="29">
         <v>19</v>
       </c>
-      <c r="C23" s="34"/>
-      <c r="D23" s="45" t="s">
+      <c r="C23" s="52"/>
+      <c r="D23" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="E23" s="42"/>
-      <c r="F23" s="37"/>
-      <c r="J23" s="55"/>
-      <c r="K23" s="61">
+      <c r="E23" s="57"/>
+      <c r="F23" s="59"/>
+      <c r="J23" s="40"/>
+      <c r="K23" s="46">
         <v>28</v>
       </c>
       <c r="L23" s="2" t="s">
         <v>125</v>
       </c>
-      <c r="M23" s="56"/>
+      <c r="M23" s="41"/>
     </row>
     <row r="24" spans="2:13">
       <c r="B24" s="29">
         <v>20</v>
       </c>
-      <c r="C24" s="34"/>
-      <c r="D24" s="45" t="s">
+      <c r="C24" s="52"/>
+      <c r="D24" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="E24" s="42"/>
-      <c r="F24" s="37"/>
-      <c r="J24" s="55"/>
-      <c r="K24" s="62">
+      <c r="E24" s="57"/>
+      <c r="F24" s="59"/>
+      <c r="J24" s="40"/>
+      <c r="K24" s="47">
         <v>6</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="M24" s="56"/>
+      <c r="M24" s="41"/>
     </row>
     <row r="25" spans="2:13">
       <c r="B25" s="29">
         <v>21</v>
       </c>
-      <c r="C25" s="35"/>
-      <c r="D25" s="45" t="s">
+      <c r="C25" s="53"/>
+      <c r="D25" s="31" t="s">
         <v>107</v>
       </c>
-      <c r="E25" s="43"/>
-      <c r="F25" s="38"/>
-      <c r="J25" s="55"/>
-      <c r="K25" s="63">
+      <c r="E25" s="58"/>
+      <c r="F25" s="60"/>
+      <c r="J25" s="40"/>
+      <c r="K25" s="48">
         <v>3</v>
       </c>
       <c r="L25" s="2" t="s">
         <v>124</v>
       </c>
-      <c r="M25" s="56"/>
+      <c r="M25" s="41"/>
     </row>
     <row r="26" spans="2:13">
       <c r="B26" s="29">
         <v>22</v>
       </c>
-      <c r="C26" s="39" t="s">
+      <c r="C26" s="61" t="s">
         <v>108</v>
       </c>
-      <c r="D26" s="46" t="s">
+      <c r="D26" s="32" t="s">
         <v>109</v>
       </c>
-      <c r="E26" s="39" t="s">
+      <c r="E26" s="61" t="s">
         <v>91</v>
       </c>
-      <c r="F26" s="40" t="s">
+      <c r="F26" s="62" t="s">
         <v>89</v>
       </c>
-      <c r="J26" s="55"/>
+      <c r="J26" s="40"/>
       <c r="K26" s="19">
         <f>SUM(K23:K25)</f>
         <v>37</v>
@@ -2338,68 +2354,68 @@
       <c r="L26" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="M26" s="56"/>
+      <c r="M26" s="41"/>
     </row>
     <row r="27" spans="2:13" ht="15" thickBot="1">
       <c r="B27" s="29">
         <v>23</v>
       </c>
-      <c r="C27" s="39"/>
-      <c r="D27" s="46" t="s">
+      <c r="C27" s="61"/>
+      <c r="D27" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="E27" s="39"/>
-      <c r="F27" s="39"/>
-      <c r="J27" s="57"/>
-      <c r="K27" s="58"/>
-      <c r="L27" s="59"/>
-      <c r="M27" s="60"/>
+      <c r="E27" s="61"/>
+      <c r="F27" s="61"/>
+      <c r="J27" s="42"/>
+      <c r="K27" s="43"/>
+      <c r="L27" s="44"/>
+      <c r="M27" s="45"/>
     </row>
     <row r="28" spans="2:13">
       <c r="B28" s="27"/>
-      <c r="C28" s="34" t="s">
+      <c r="C28" s="52" t="s">
         <v>110</v>
       </c>
-      <c r="D28" s="44" t="s">
+      <c r="D28" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="E28" s="33" t="s">
+      <c r="E28" s="54" t="s">
         <v>110</v>
       </c>
-      <c r="F28" s="36" t="s">
+      <c r="F28" s="55" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="29" spans="2:13">
       <c r="B29" s="27"/>
-      <c r="C29" s="34"/>
-      <c r="D29" s="44" t="s">
+      <c r="C29" s="52"/>
+      <c r="D29" s="30" t="s">
         <v>112</v>
       </c>
-      <c r="E29" s="34"/>
-      <c r="F29" s="34"/>
+      <c r="E29" s="52"/>
+      <c r="F29" s="52"/>
     </row>
     <row r="30" spans="2:13">
       <c r="B30" s="27"/>
-      <c r="C30" s="34"/>
-      <c r="D30" s="44" t="s">
+      <c r="C30" s="52"/>
+      <c r="D30" s="30" t="s">
         <v>113</v>
       </c>
-      <c r="E30" s="35"/>
-      <c r="F30" s="35"/>
+      <c r="E30" s="53"/>
+      <c r="F30" s="53"/>
     </row>
     <row r="31" spans="2:13">
       <c r="B31" s="29">
         <v>24</v>
       </c>
-      <c r="C31" s="34"/>
-      <c r="D31" s="46" t="s">
+      <c r="C31" s="52"/>
+      <c r="D31" s="32" t="s">
         <v>126</v>
       </c>
-      <c r="E31" s="33" t="s">
+      <c r="E31" s="54" t="s">
         <v>91</v>
       </c>
-      <c r="F31" s="36" t="s">
+      <c r="F31" s="55" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2407,38 +2423,38 @@
       <c r="B32" s="28">
         <v>25</v>
       </c>
-      <c r="C32" s="34"/>
-      <c r="D32" s="46" t="s">
+      <c r="C32" s="52"/>
+      <c r="D32" s="32" t="s">
         <v>127</v>
       </c>
-      <c r="E32" s="34"/>
-      <c r="F32" s="34"/>
+      <c r="E32" s="52"/>
+      <c r="F32" s="52"/>
     </row>
     <row r="33" spans="2:6">
       <c r="B33" s="29">
         <v>26</v>
       </c>
-      <c r="C33" s="35"/>
-      <c r="D33" s="46" t="s">
+      <c r="C33" s="53"/>
+      <c r="D33" s="32" t="s">
         <v>128</v>
       </c>
-      <c r="E33" s="35"/>
-      <c r="F33" s="35"/>
+      <c r="E33" s="53"/>
+      <c r="F33" s="53"/>
     </row>
     <row r="34" spans="2:6">
       <c r="B34" s="29">
         <v>27</v>
       </c>
-      <c r="C34" s="33" t="s">
+      <c r="C34" s="54" t="s">
         <v>115</v>
       </c>
-      <c r="D34" s="46" t="s">
+      <c r="D34" s="32" t="s">
         <v>63</v>
       </c>
-      <c r="E34" s="33" t="s">
+      <c r="E34" s="54" t="s">
         <v>91</v>
       </c>
-      <c r="F34" s="36" t="s">
+      <c r="F34" s="55" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2446,71 +2462,71 @@
       <c r="B35" s="29">
         <v>28</v>
       </c>
-      <c r="C35" s="34"/>
-      <c r="D35" s="46" t="s">
+      <c r="C35" s="52"/>
+      <c r="D35" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="E35" s="34"/>
-      <c r="F35" s="37"/>
+      <c r="E35" s="52"/>
+      <c r="F35" s="59"/>
     </row>
     <row r="36" spans="2:6">
       <c r="B36" s="29">
         <v>29</v>
       </c>
-      <c r="C36" s="34"/>
-      <c r="D36" s="46" t="s">
+      <c r="C36" s="52"/>
+      <c r="D36" s="32" t="s">
         <v>116</v>
       </c>
-      <c r="E36" s="34"/>
-      <c r="F36" s="37"/>
+      <c r="E36" s="52"/>
+      <c r="F36" s="59"/>
     </row>
     <row r="37" spans="2:6">
       <c r="B37" s="29">
         <v>30</v>
       </c>
-      <c r="C37" s="34"/>
-      <c r="D37" s="46" t="s">
+      <c r="C37" s="52"/>
+      <c r="D37" s="32" t="s">
         <v>62</v>
       </c>
-      <c r="E37" s="34"/>
-      <c r="F37" s="37"/>
+      <c r="E37" s="52"/>
+      <c r="F37" s="59"/>
     </row>
     <row r="38" spans="2:6">
       <c r="B38" s="29">
         <v>31</v>
       </c>
-      <c r="C38" s="34"/>
-      <c r="D38" s="46" t="s">
+      <c r="C38" s="52"/>
+      <c r="D38" s="32" t="s">
         <v>121</v>
       </c>
-      <c r="E38" s="34"/>
-      <c r="F38" s="37"/>
+      <c r="E38" s="52"/>
+      <c r="F38" s="59"/>
     </row>
     <row r="39" spans="2:6">
       <c r="B39" s="29">
         <v>32</v>
       </c>
-      <c r="C39" s="35"/>
-      <c r="D39" s="46" t="s">
+      <c r="C39" s="53"/>
+      <c r="D39" s="32" t="s">
         <v>117</v>
       </c>
-      <c r="E39" s="35"/>
-      <c r="F39" s="38"/>
+      <c r="E39" s="53"/>
+      <c r="F39" s="60"/>
     </row>
     <row r="40" spans="2:6">
       <c r="B40" s="29">
         <v>33</v>
       </c>
-      <c r="C40" s="50" t="s">
+      <c r="C40" s="63" t="s">
         <v>118</v>
       </c>
-      <c r="D40" s="46" t="s">
+      <c r="D40" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="E40" s="33" t="s">
+      <c r="E40" s="54" t="s">
         <v>91</v>
       </c>
-      <c r="F40" s="36" t="s">
+      <c r="F40" s="55" t="s">
         <v>89</v>
       </c>
     </row>
@@ -2518,51 +2534,51 @@
       <c r="B41" s="29">
         <v>34</v>
       </c>
-      <c r="C41" s="50"/>
-      <c r="D41" s="46" t="s">
+      <c r="C41" s="63"/>
+      <c r="D41" s="32" t="s">
         <v>56</v>
       </c>
-      <c r="E41" s="34"/>
-      <c r="F41" s="37"/>
+      <c r="E41" s="52"/>
+      <c r="F41" s="59"/>
     </row>
     <row r="42" spans="2:6">
       <c r="B42" s="29">
         <v>35</v>
       </c>
-      <c r="C42" s="50"/>
-      <c r="D42" s="46" t="s">
+      <c r="C42" s="63"/>
+      <c r="D42" s="32" t="s">
         <v>60</v>
       </c>
-      <c r="E42" s="34"/>
-      <c r="F42" s="37"/>
+      <c r="E42" s="52"/>
+      <c r="F42" s="59"/>
     </row>
     <row r="43" spans="2:6">
       <c r="B43" s="29">
         <v>36</v>
       </c>
-      <c r="C43" s="50"/>
-      <c r="D43" s="46" t="s">
+      <c r="C43" s="63"/>
+      <c r="D43" s="32" t="s">
         <v>119</v>
       </c>
-      <c r="E43" s="34"/>
-      <c r="F43" s="37"/>
+      <c r="E43" s="52"/>
+      <c r="F43" s="59"/>
     </row>
     <row r="44" spans="2:6">
       <c r="B44" s="29">
         <v>37</v>
       </c>
-      <c r="C44" s="50"/>
-      <c r="D44" s="46" t="s">
+      <c r="C44" s="63"/>
+      <c r="D44" s="32" t="s">
         <v>120</v>
       </c>
-      <c r="E44" s="34"/>
-      <c r="F44" s="37"/>
+      <c r="E44" s="52"/>
+      <c r="F44" s="59"/>
     </row>
     <row r="45" spans="2:6">
       <c r="B45" s="28"/>
-      <c r="C45" s="49"/>
+      <c r="C45" s="35"/>
       <c r="D45" s="23"/>
-      <c r="E45" s="48"/>
+      <c r="E45" s="34"/>
       <c r="F45" s="2"/>
     </row>
     <row r="46" spans="2:6">
@@ -2602,6 +2618,18 @@
     </row>
   </sheetData>
   <mergeCells count="23">
+    <mergeCell ref="E34:E39"/>
+    <mergeCell ref="F34:F39"/>
+    <mergeCell ref="C34:C39"/>
+    <mergeCell ref="F40:F44"/>
+    <mergeCell ref="E40:E44"/>
+    <mergeCell ref="C40:C44"/>
+    <mergeCell ref="C5:C11"/>
+    <mergeCell ref="C12:C14"/>
+    <mergeCell ref="E5:E14"/>
+    <mergeCell ref="F5:F14"/>
+    <mergeCell ref="E15:E19"/>
+    <mergeCell ref="F15:F19"/>
     <mergeCell ref="C28:C33"/>
     <mergeCell ref="E31:E33"/>
     <mergeCell ref="F28:F30"/>
@@ -2609,22 +2637,10 @@
     <mergeCell ref="E20:E25"/>
     <mergeCell ref="F20:F25"/>
     <mergeCell ref="C15:C25"/>
-    <mergeCell ref="C5:C11"/>
-    <mergeCell ref="C12:C14"/>
-    <mergeCell ref="E5:E14"/>
-    <mergeCell ref="F5:F14"/>
-    <mergeCell ref="E15:E19"/>
-    <mergeCell ref="F15:F19"/>
     <mergeCell ref="C26:C27"/>
     <mergeCell ref="E26:E27"/>
     <mergeCell ref="F26:F27"/>
     <mergeCell ref="E28:E30"/>
-    <mergeCell ref="E34:E39"/>
-    <mergeCell ref="F34:F39"/>
-    <mergeCell ref="C34:C39"/>
-    <mergeCell ref="F40:F44"/>
-    <mergeCell ref="E40:E44"/>
-    <mergeCell ref="C40:C44"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="F5" r:id="rId1"/>
@@ -2643,12 +2659,94 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="C4:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
-  <sheetData/>
+  <cols>
+    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:4">
+      <c r="C4" s="64" t="s">
+        <v>131</v>
+      </c>
+      <c r="D4" s="64" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="5" spans="3:4">
+      <c r="C5" s="2" t="s">
+        <v>134</v>
+      </c>
+      <c r="D5" s="2"/>
+    </row>
+    <row r="6" spans="3:4">
+      <c r="C6" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="3:4">
+      <c r="C7" s="2"/>
+      <c r="D7" s="2"/>
+    </row>
+    <row r="8" spans="3:4">
+      <c r="C8" s="2"/>
+      <c r="D8" s="2"/>
+    </row>
+    <row r="9" spans="3:4">
+      <c r="C9" s="2"/>
+      <c r="D9" s="2"/>
+    </row>
+    <row r="10" spans="3:4">
+      <c r="C10" s="2"/>
+      <c r="D10" s="2"/>
+    </row>
+    <row r="11" spans="3:4">
+      <c r="C11" s="2"/>
+      <c r="D11" s="2"/>
+    </row>
+    <row r="12" spans="3:4">
+      <c r="C12" s="2"/>
+      <c r="D12" s="2"/>
+    </row>
+    <row r="13" spans="3:4">
+      <c r="C13" s="2"/>
+      <c r="D13" s="2"/>
+    </row>
+    <row r="14" spans="3:4">
+      <c r="C14" s="2"/>
+      <c r="D14" s="2"/>
+    </row>
+    <row r="15" spans="3:4">
+      <c r="C15" s="2"/>
+      <c r="D15" s="2"/>
+    </row>
+    <row r="16" spans="3:4">
+      <c r="C16" s="2"/>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="3:4">
+      <c r="C17" s="2"/>
+      <c r="D17" s="2"/>
+    </row>
+    <row r="18" spans="3:4">
+      <c r="C18" s="2"/>
+      <c r="D18" s="2"/>
+    </row>
+    <row r="19" spans="3:4">
+      <c r="C19" s="2"/>
+      <c r="D19" s="2"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>